<commit_message>
doku 4 seiten fertig
</commit_message>
<xml_diff>
--- a/Doku/EnergieVerlustVergleich.xlsx
+++ b/Doku/EnergieVerlustVergleich.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git-Repos\simulation\Auswertungen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\3 Schule\Next\Doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64D2E36-E952-4A99-9D48-0BDB462BDFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vergleich" sheetId="1" r:id="rId1"/>
     <sheet name="NASA Vergleich" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="36">
   <si>
     <t>Euler:</t>
   </si>
@@ -125,11 +126,20 @@
   <si>
     <t>-1,766E-11%</t>
   </si>
+  <si>
+    <t>DKD leapfrog</t>
+  </si>
+  <si>
+    <t>KDK leapfrog</t>
+  </si>
+  <si>
+    <t>Runge Kutta (RK4)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000%"/>
@@ -209,7 +219,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,6 +244,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -430,7 +446,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -477,8 +493,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="7" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="7" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="7" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="7" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="7" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Ausgabe" xfId="6" builtinId="21"/>
@@ -798,30 +818,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AB31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:AA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J47" sqref="D31:J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" customWidth="1"/>
     <col min="11" max="11" width="23.140625" customWidth="1"/>
     <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23" customWidth="1"/>
+    <col min="14" max="14" width="23.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" customWidth="1"/>
     <col min="22" max="22" width="14" customWidth="1"/>
     <col min="23" max="23" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:28" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
@@ -846,8 +868,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -865,17 +887,17 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="R7" s="5"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C8" s="4"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C9" s="4"/>
       <c r="D9" t="s">
         <v>3</v>
@@ -923,7 +945,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C10" s="4"/>
       <c r="D10">
         <v>10</v>
@@ -947,7 +969,6 @@
       <c r="M10" s="40">
         <v>-8.5000000000000006E-3</v>
       </c>
-      <c r="N10" s="42"/>
       <c r="P10">
         <v>10</v>
       </c>
@@ -963,12 +984,13 @@
       <c r="U10">
         <v>100000</v>
       </c>
+      <c r="V10" s="8">
+        <v>1.9E+25</v>
+      </c>
       <c r="W10" s="41"/>
-      <c r="X10" s="42"/>
       <c r="AA10" s="40"/>
-      <c r="AB10" s="42"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C11" s="4"/>
       <c r="D11">
         <v>100</v>
@@ -991,7 +1013,7 @@
       <c r="M11" s="40">
         <v>-1E-3</v>
       </c>
-      <c r="N11" s="42">
+      <c r="N11">
         <v>792</v>
       </c>
       <c r="P11">
@@ -1015,14 +1037,13 @@
       <c r="W11" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="X11" s="42">
+      <c r="X11">
         <v>396</v>
       </c>
       <c r="Z11" s="8"/>
       <c r="AA11" s="8"/>
-      <c r="AB11" s="42"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C12" s="4"/>
       <c r="D12">
         <v>1000</v>
@@ -1045,7 +1066,7 @@
       <c r="M12" s="40">
         <v>-1E-4</v>
       </c>
-      <c r="N12" s="42">
+      <c r="N12">
         <v>7992</v>
       </c>
       <c r="P12">
@@ -1063,14 +1084,14 @@
       <c r="U12">
         <v>1000</v>
       </c>
-      <c r="V12" s="8"/>
+      <c r="V12" s="8">
+        <v>7.6599999999999995E+23</v>
+      </c>
       <c r="W12" s="41"/>
-      <c r="X12" s="42"/>
       <c r="Z12" s="8"/>
       <c r="AA12" s="40"/>
-      <c r="AB12" s="42"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C13" s="4"/>
       <c r="D13">
         <v>10000</v>
@@ -1093,7 +1114,7 @@
       <c r="M13" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="N13" s="42">
+      <c r="N13">
         <v>79992</v>
       </c>
       <c r="P13">
@@ -1117,14 +1138,13 @@
       <c r="W13" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="X13" s="42">
+      <c r="X13">
         <v>39996</v>
       </c>
       <c r="Z13" s="8"/>
       <c r="AA13" s="41"/>
-      <c r="AB13" s="42"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C14" s="4"/>
       <c r="D14">
         <v>100000</v>
@@ -1153,7 +1173,7 @@
       <c r="M14" s="41">
         <v>-9.9999999999999995E-7</v>
       </c>
-      <c r="N14" s="42">
+      <c r="N14">
         <v>799992</v>
       </c>
       <c r="P14">
@@ -1177,14 +1197,13 @@
       <c r="W14" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="X14" s="42">
+      <c r="X14">
         <v>399996</v>
       </c>
       <c r="Z14" s="8"/>
       <c r="AA14" s="41"/>
-      <c r="AB14" s="42"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C15" s="4"/>
       <c r="D15">
         <v>1000000</v>
@@ -1207,7 +1226,7 @@
       <c r="M15" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="N15" s="42">
+      <c r="N15">
         <v>7999992</v>
       </c>
       <c r="P15">
@@ -1231,11 +1250,11 @@
       <c r="W15" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="X15" s="42">
+      <c r="X15">
         <v>3999996</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
@@ -1246,7 +1265,7 @@
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
-      <c r="M16" s="43"/>
+      <c r="M16" s="11"/>
       <c r="N16" s="11"/>
       <c r="O16" s="11"/>
       <c r="P16" s="11"/>
@@ -1444,25 +1463,443 @@
       <c r="R26" s="12"/>
     </row>
     <row r="30" spans="3:18" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" t="s">
+        <v>2</v>
+      </c>
+      <c r="J32" t="s">
+        <v>4</v>
+      </c>
+      <c r="L32" t="s">
+        <v>3</v>
+      </c>
+      <c r="M32" t="s">
+        <v>2</v>
+      </c>
+      <c r="N32" t="s">
+        <v>4</v>
+      </c>
+      <c r="P32" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>2</v>
+      </c>
+      <c r="R32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <v>100000</v>
+      </c>
+      <c r="F33" s="46">
+        <v>-8.6368983495103798E+30</v>
+      </c>
+      <c r="H33">
+        <v>10</v>
+      </c>
+      <c r="I33">
+        <v>100000</v>
+      </c>
+      <c r="J33">
+        <f>-2.29E+31</f>
+        <v>-2.29E+31</v>
+      </c>
+      <c r="L33">
+        <v>10</v>
+      </c>
+      <c r="M33">
+        <v>100000</v>
+      </c>
+      <c r="N33" s="42">
+        <v>3.3018388667247001E+27</v>
+      </c>
+      <c r="P33">
+        <v>10</v>
+      </c>
+      <c r="Q33">
+        <v>100000</v>
+      </c>
+      <c r="R33" s="8">
+        <v>1.9E+25</v>
+      </c>
+    </row>
+    <row r="34" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>100</v>
+      </c>
+      <c r="E34">
+        <v>10000</v>
+      </c>
+      <c r="F34" s="46">
+        <v>-1.05465784151321E+30</v>
+      </c>
+      <c r="H34">
+        <v>100</v>
+      </c>
+      <c r="I34">
+        <v>10000</v>
+      </c>
+      <c r="J34" s="8">
+        <v>-2.7900000000000001E+30</v>
+      </c>
+      <c r="L34">
+        <v>100</v>
+      </c>
+      <c r="M34">
+        <v>10000</v>
+      </c>
+      <c r="N34" s="44">
+        <v>-2.5090178695766899E+26</v>
+      </c>
+      <c r="P34">
+        <v>100</v>
+      </c>
+      <c r="Q34">
+        <v>10000</v>
+      </c>
+      <c r="R34" s="8">
+        <v>5.2200000000000002E+24</v>
+      </c>
+    </row>
+    <row r="35" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>1000</v>
+      </c>
+      <c r="E35">
+        <v>1000</v>
+      </c>
+      <c r="F35" s="46">
+        <v>-1.0764205093716899E+29</v>
+      </c>
+      <c r="H35">
+        <v>1000</v>
+      </c>
+      <c r="I35">
+        <v>1000</v>
+      </c>
+      <c r="J35" s="8">
+        <v>-2.84E+29</v>
+      </c>
+      <c r="L35">
+        <v>1000</v>
+      </c>
+      <c r="M35">
+        <v>1000</v>
+      </c>
+      <c r="N35" s="43">
+        <v>-3.1410744913864503E+26</v>
+      </c>
+      <c r="P35">
+        <v>1000</v>
+      </c>
+      <c r="Q35">
+        <v>1000</v>
+      </c>
+      <c r="R35" s="8">
+        <v>7.6599999999999995E+23</v>
+      </c>
+    </row>
+    <row r="36" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>10000</v>
+      </c>
+      <c r="E36">
+        <v>100</v>
+      </c>
+      <c r="F36" s="47">
+        <v>-1.1067427619372699E+28</v>
+      </c>
+      <c r="H36">
+        <v>10000</v>
+      </c>
+      <c r="I36">
+        <v>100</v>
+      </c>
+      <c r="J36" s="8">
+        <v>-2.8799999999999999E+28</v>
+      </c>
+      <c r="L36">
+        <v>10000</v>
+      </c>
+      <c r="M36">
+        <v>100</v>
+      </c>
+      <c r="N36" s="43">
+        <v>-3.1577904120513702E+26</v>
+      </c>
+      <c r="P36">
+        <v>10000</v>
+      </c>
+      <c r="Q36">
+        <v>100</v>
+      </c>
+      <c r="R36" s="8">
+        <v>6.4199999999999998E+22</v>
+      </c>
+    </row>
+    <row r="37" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>100000</v>
+      </c>
+      <c r="E37">
+        <v>10</v>
+      </c>
+      <c r="F37" s="47">
+        <v>-1.39125116563088E+27</v>
+      </c>
+      <c r="H37">
+        <v>100000</v>
+      </c>
+      <c r="I37">
+        <v>10</v>
+      </c>
+      <c r="J37" s="8">
+        <v>-3.17E+27</v>
+      </c>
+      <c r="L37">
+        <v>100000</v>
+      </c>
+      <c r="M37">
+        <v>10</v>
+      </c>
+      <c r="N37" s="43">
+        <v>-3.1589778693196503E+26</v>
+      </c>
+      <c r="P37">
+        <v>100000</v>
+      </c>
+      <c r="Q37">
+        <v>10</v>
+      </c>
+      <c r="R37" s="8">
+        <v>6.2700000000000005E+21</v>
+      </c>
+    </row>
+    <row r="38" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>1000000</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" s="45">
+        <v>-4.2344627093166798E+26</v>
+      </c>
+      <c r="H38">
+        <v>1000000</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38" s="8">
+        <v>-6.0569999999999999E+26</v>
+      </c>
+      <c r="L38">
+        <v>1000000</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38" s="43">
+        <v>-3.1589778693196503E+26</v>
+      </c>
+      <c r="P38">
+        <v>1000000</v>
+      </c>
+      <c r="Q38">
+        <v>1</v>
+      </c>
+      <c r="R38" s="8">
+        <v>4.715E+20</v>
+      </c>
+    </row>
+    <row r="39" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="F39" s="45"/>
+      <c r="J39" s="8"/>
+      <c r="N39" s="43"/>
+      <c r="R39" s="8"/>
+    </row>
+    <row r="40" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>33</v>
+      </c>
+      <c r="H40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" t="s">
+        <v>4</v>
+      </c>
+      <c r="H41" t="s">
+        <v>3</v>
+      </c>
+      <c r="I41" t="s">
+        <v>2</v>
+      </c>
+      <c r="J41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>10</v>
+      </c>
+      <c r="E42">
+        <v>100000</v>
+      </c>
+      <c r="F42" s="42">
+        <v>3.3018388667247001E+27</v>
+      </c>
+      <c r="H42">
+        <v>10</v>
+      </c>
+      <c r="I42">
+        <v>100000</v>
+      </c>
+      <c r="J42" s="8">
+        <v>1.9E+25</v>
+      </c>
+    </row>
+    <row r="43" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>100</v>
+      </c>
+      <c r="E43">
+        <v>10000</v>
+      </c>
+      <c r="F43" s="44">
+        <v>-2.5090178695766899E+26</v>
+      </c>
+      <c r="H43">
+        <v>100</v>
+      </c>
+      <c r="I43">
+        <v>10000</v>
+      </c>
+      <c r="J43" s="8">
+        <v>5.2200000000000002E+24</v>
+      </c>
+    </row>
+    <row r="44" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>1000</v>
+      </c>
+      <c r="E44">
+        <v>1000</v>
+      </c>
+      <c r="F44" s="43">
+        <v>-3.1410744913864503E+26</v>
+      </c>
+      <c r="H44">
+        <v>1000</v>
+      </c>
+      <c r="I44">
+        <v>1000</v>
+      </c>
+      <c r="J44" s="8">
+        <v>7.6599999999999995E+23</v>
+      </c>
+    </row>
+    <row r="45" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>10000</v>
+      </c>
+      <c r="E45">
+        <v>100</v>
+      </c>
+      <c r="F45" s="43">
+        <v>-3.1577904120513702E+26</v>
+      </c>
+      <c r="H45">
+        <v>10000</v>
+      </c>
+      <c r="I45">
+        <v>100</v>
+      </c>
+      <c r="J45" s="8">
+        <v>6.4199999999999998E+22</v>
+      </c>
+    </row>
+    <row r="46" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>100000</v>
+      </c>
+      <c r="E46">
+        <v>10</v>
+      </c>
+      <c r="F46" s="43">
+        <v>-3.1589778693196503E+26</v>
+      </c>
+      <c r="H46">
+        <v>100000</v>
+      </c>
+      <c r="I46">
+        <v>10</v>
+      </c>
+      <c r="J46" s="8">
+        <v>6.2700000000000005E+21</v>
+      </c>
+    </row>
+    <row r="47" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>1000000</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" s="43">
+        <v>-3.1589778693196503E+26</v>
+      </c>
+      <c r="H47">
+        <v>1000000</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47" s="8">
+        <v>4.715E+20</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F22:F25">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="F42:F47">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q22:Q25">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
+        <color theme="0"/>
+        <color theme="0"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -1472,7 +1909,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X61"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
@@ -3097,6 +3534,18 @@
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H57 F57 R57 T57 R44 T44 F44 H44 F18 H18 R18">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -3140,18 +3589,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F57 H57 R57 T57 R44 T44 F44 H44 F18 H18 R18">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
energie verlust in doku fertig
</commit_message>
<xml_diff>
--- a/Doku/EnergieVerlustVergleich.xlsx
+++ b/Doku/EnergieVerlustVergleich.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\3 Schule\Next\Doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3837C682-9E3B-457B-BDF4-DE1B60D59816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6F2E2A-56DF-48D4-8D5F-423A05664D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Vergleich" sheetId="1" r:id="rId1"/>
-    <sheet name="NASA Vergleich" sheetId="2" r:id="rId2"/>
+    <sheet name="Diagramm1" sheetId="3" r:id="rId1"/>
+    <sheet name="Vergleich" sheetId="1" r:id="rId2"/>
+    <sheet name="NASA Vergleich" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -569,18 +570,264 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="557658984"/>
+        <c:axId val="557655744"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="557658984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="557655744"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="557655744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="557658984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Numerische Methoden Energieverlust</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v> Euler</c:v>
+          </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
+              <a:headEnd type="none"/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -656,260 +903,22 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-83EE-414F-9C4F-D36C62B5C0C2}"/>
+              <c16:uniqueId val="{00000000-378A-4047-AEA6-01ACE09715D9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="999971232"/>
-        <c:axId val="999966912"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="999971232"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>KDK leapfrog</c:v>
+          </c:tx>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="999966912"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="999966912"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="999971232"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="1.9895099104728586E-2"/>
-          <c:y val="7.8850812380938551E-2"/>
-          <c:w val="0.92956045009631227"/>
-          <c:h val="0.77765546644301164"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -919,11 +928,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -958,45 +967,48 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Vergleich!$G$33:$G$38</c:f>
+              <c:f>Vergleich!$G$42:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>8.6368983495103798E+30</c:v>
+                  <c:v>3.3018388667247001E+27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.05465784151321E+30</c:v>
+                  <c:v>2.5090178695766899E+26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0764205093716899E+29</c:v>
+                  <c:v>3.1410744913864503E+26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1067427619372699E+28</c:v>
+                  <c:v>3.1577904120513702E+26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.39125116563088E+27</c:v>
+                  <c:v>3.1589778693196503E+26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.2344627093166798E+26</c:v>
+                  <c:v>3.1589778693196503E+26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-77A5-43D8-AF17-966CDC7108A0}"/>
+              <c16:uniqueId val="{00000001-378A-4047-AEA6-01ACE09715D9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Runge Kutta</c:v>
+          </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1007,11 +1019,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1071,10 +1083,105 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-77A5-43D8-AF17-966CDC7108A0}"/>
+              <c16:uniqueId val="{00000002-378A-4047-AEA6-01ACE09715D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>DKD leapfrog</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="lgDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Vergleich!$E$33:$E$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Vergleich!$J$42:$J$47</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.9E+25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2200000000000002E+24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.6599999999999995E+23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.4199999999999998E+22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.2700000000000005E+21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.715E+20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-378A-4047-AEA6-01ACE09715D9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1086,11 +1193,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1005668160"/>
-        <c:axId val="1005671040"/>
+        <c:axId val="647410896"/>
+        <c:axId val="647415216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1005668160"/>
+        <c:axId val="647410896"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1111,6 +1218,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>deltaTime in s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1148,16 +1310,16 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1005671040"/>
+        <c:crossAx val="647415216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1005671040"/>
+        <c:axId val="647415216"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:min val="9.9999999999999988E+25"/>
+          <c:min val="1E+20"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1175,6 +1337,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t>Energieverlust in J</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1212,7 +1430,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1005668160"/>
+        <c:crossAx val="647410896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1225,7 +1443,17 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.84899360684891567"/>
+          <c:y val="9.2008861669910014E-2"/>
+          <c:w val="0.12722710470085205"/>
+          <c:h val="0.71471869490021001"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1257,6 +1485,13 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1373,7 +1608,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1400,8 +1635,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1502,7 +1737,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1534,10 +1769,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1577,23 +1812,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1698,8 +1932,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1831,20 +2065,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1858,17 +2091,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2404,27 +2626,71 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{002ECBCF-B915-4AAC-BC62-EB09F0667A50}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>138872</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>185217</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>329372</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>84524</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9308171" cy="6017012"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B06FFFA-C6BC-3963-9176-F701BA4F475A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45F61C99-A465-24D5-E320-A7B68F5E22BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>415637</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>51955</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B02B23B0-1605-CC3D-C6BB-19A6209E9399}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2437,42 +2703,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>16807</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>67235</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>593910</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>54908</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C040EA89-FA68-C870-AD5D-BAC0B0B636DD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2780,8 +3010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K33" activeCellId="2" sqref="E33:E38 G33:G38 K33:K38"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AE53" sqref="AE53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3526,7 +3756,7 @@
         <v>-1.05465784151321E+30</v>
       </c>
       <c r="G34" s="8">
-        <f t="shared" ref="G34:G38" si="0">F34*-1</f>
+        <f t="shared" ref="G34:G47" si="0">F34*-1</f>
         <v>1.05465784151321E+30</v>
       </c>
       <c r="H34">
@@ -3747,6 +3977,10 @@
     </row>
     <row r="39" spans="4:18" x14ac:dyDescent="0.25">
       <c r="F39" s="45"/>
+      <c r="G39" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="J39" s="8"/>
       <c r="N39" s="43"/>
       <c r="R39" s="8"/>
@@ -3755,6 +3989,10 @@
       <c r="D40" t="s">
         <v>33</v>
       </c>
+      <c r="G40" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H40" t="s">
         <v>34</v>
       </c>
@@ -3769,6 +4007,10 @@
       <c r="F41" t="s">
         <v>4</v>
       </c>
+      <c r="G41" s="8" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="H41" t="s">
         <v>3</v>
       </c>
@@ -3789,6 +4031,10 @@
       <c r="F42" s="42">
         <v>3.3018388667247001E+27</v>
       </c>
+      <c r="G42" s="8">
+        <f>F42</f>
+        <v>3.3018388667247001E+27</v>
+      </c>
       <c r="H42">
         <v>10</v>
       </c>
@@ -3809,6 +4055,10 @@
       <c r="F43" s="44">
         <v>-2.5090178695766899E+26</v>
       </c>
+      <c r="G43" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5090178695766899E+26</v>
+      </c>
       <c r="H43">
         <v>100</v>
       </c>
@@ -3829,6 +4079,10 @@
       <c r="F44" s="43">
         <v>-3.1410744913864503E+26</v>
       </c>
+      <c r="G44" s="8">
+        <f t="shared" si="0"/>
+        <v>3.1410744913864503E+26</v>
+      </c>
       <c r="H44">
         <v>1000</v>
       </c>
@@ -3849,6 +4103,10 @@
       <c r="F45" s="43">
         <v>-3.1577904120513702E+26</v>
       </c>
+      <c r="G45" s="8">
+        <f t="shared" si="0"/>
+        <v>3.1577904120513702E+26</v>
+      </c>
       <c r="H45">
         <v>10000</v>
       </c>
@@ -3869,6 +4127,10 @@
       <c r="F46" s="43">
         <v>-3.1589778693196503E+26</v>
       </c>
+      <c r="G46" s="8">
+        <f t="shared" si="0"/>
+        <v>3.1589778693196503E+26</v>
+      </c>
       <c r="H46">
         <v>100000</v>
       </c>
@@ -3888,6 +4150,10 @@
       </c>
       <c r="F47" s="43">
         <v>-3.1589778693196503E+26</v>
+      </c>
+      <c r="G47" s="8">
+        <f t="shared" si="0"/>
+        <v>3.1589778693196503E+26</v>
       </c>
       <c r="H47">
         <v>1000000</v>
@@ -5505,18 +5771,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F57 H57 R57 T57 R44 T44 F44 H44 F18 H18 R18">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F18:H18">
     <cfRule type="colorScale" priority="9">
       <colorScale>
@@ -5554,6 +5808,18 @@
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H57 F57 R57 T57 R44 T44 F44 H44 F18 H18 R18">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>